<commit_message>
2022 08 12 16:09
</commit_message>
<xml_diff>
--- a/assets/datamentah.xlsx
+++ b/assets/datamentah.xlsx
@@ -21,7 +21,7 @@
     <sheet name="clear" sheetId="4" r:id="rId7"/>
     <sheet name="produk" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="227">
   <si>
     <t>id_bank</t>
   </si>
@@ -633,9 +633,6 @@
     <t>200                                 </t>
   </si>
   <si>
-    <t>2022-07-17JANE.png</t>
-  </si>
-  <si>
     <t>nama_produk</t>
   </si>
   <si>
@@ -655,12 +652,72 @@
   </si>
   <si>
     <t>harga_produk</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dovpo panda.jpg</t>
+  </si>
+  <si>
+    <t>aegis legend.jpg</t>
+  </si>
+  <si>
+    <t>caliburn.jpg</t>
+  </si>
+  <si>
+    <t>druga squonk.jpg</t>
+  </si>
+  <si>
+    <t>exceed grip.jpg</t>
+  </si>
+  <si>
+    <t>hexohm v3.jpg</t>
+  </si>
+  <si>
+    <t>juul.jpg</t>
+  </si>
+  <si>
+    <t>smok fetch mini.jpg</t>
+  </si>
+  <si>
+    <t>pico75watt.jpg</t>
+  </si>
+  <si>
+    <t>smoant tc 218.jpg</t>
+  </si>
+  <si>
+    <t>smok rpm40.jpg</t>
+  </si>
+  <si>
+    <t>suorinair.jpg</t>
+  </si>
+  <si>
+    <t>tesla terminator.jpg</t>
+  </si>
+  <si>
+    <t>vaporite mecha kit 22.jpg</t>
+  </si>
+  <si>
+    <t>voopoo drag 2.jpg</t>
+  </si>
+  <si>
+    <t>zoo pod.jpg</t>
+  </si>
+  <si>
+    <t>Upods Cube,jpg</t>
+  </si>
+  <si>
+    <t>Art Mod by Preva x Owlexandrea.jpg</t>
+  </si>
+  <si>
+    <t>Mecha Kit AV Timekeeper Revolver Kit.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -3779,10 +3836,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3792,40 +3849,41 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="15" t="s">
         <v>173</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>206</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>207</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60">
+    <row r="2" spans="1:11" ht="45">
       <c r="A2" s="14">
         <v>2</v>
       </c>
@@ -3845,7 +3903,7 @@
         <v>179</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>178</v>
+        <v>208</v>
       </c>
       <c r="H2" s="14">
         <v>20000</v>
@@ -3853,8 +3911,12 @@
       <c r="I2" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="45">
+      <c r="K2" t="str">
+        <f>"UPDATE produk SET gambar = '"&amp;G2&amp;"' WHERE id_produk = "&amp;A2&amp;";"</f>
+        <v>UPDATE produk SET gambar = 'dovpo panda.jpg' WHERE id_produk = 2;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30">
       <c r="A3" s="14">
         <v>3</v>
       </c>
@@ -3871,10 +3933,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="H3" s="14">
         <v>30000</v>
@@ -3882,8 +3944,12 @@
       <c r="I3" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="30">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K30" si="0">"UPDATE produk SET gambar = '"&amp;G3&amp;"' WHERE id_produk = "&amp;A3&amp;";"</f>
+        <v>UPDATE produk SET gambar = 'exceed grip.jpg' WHERE id_produk = 3;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="14">
         <v>4</v>
       </c>
@@ -3903,7 +3969,7 @@
         <v>179</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>181</v>
+        <v>224</v>
       </c>
       <c r="H4" s="14">
         <v>40000</v>
@@ -3911,8 +3977,12 @@
       <c r="I4" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="60">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'Upods Cube,jpg' WHERE id_produk = 4;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45">
       <c r="A5" s="14">
         <v>5</v>
       </c>
@@ -3932,7 +4002,7 @@
         <v>179</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>182</v>
+        <v>221</v>
       </c>
       <c r="H5" s="14">
         <v>50000</v>
@@ -3940,8 +4010,12 @@
       <c r="I5" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="105">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'vaporite mecha kit 22.jpg' WHERE id_produk = 5;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="75">
       <c r="A6" s="14">
         <v>6</v>
       </c>
@@ -3961,7 +4035,7 @@
         <v>179</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
       <c r="H6" s="14">
         <v>60000</v>
@@ -3969,8 +4043,12 @@
       <c r="I6" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="30">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'hexohm v3.jpg' WHERE id_produk = 6;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="14">
         <v>7</v>
       </c>
@@ -3990,7 +4068,7 @@
         <v>179</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="H7" s="14">
         <v>70000</v>
@@ -3998,8 +4076,12 @@
       <c r="I7" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="45">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'juul.jpg' WHERE id_produk = 7;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="14">
         <v>8</v>
       </c>
@@ -4019,7 +4101,7 @@
         <v>179</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>185</v>
+        <v>215</v>
       </c>
       <c r="H8" s="14">
         <v>80000</v>
@@ -4027,8 +4109,12 @@
       <c r="I8" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="75">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'smok fetch mini.jpg' WHERE id_produk = 8;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60">
       <c r="A9" s="14">
         <v>9</v>
       </c>
@@ -4048,7 +4134,7 @@
         <v>179</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>186</v>
+        <v>225</v>
       </c>
       <c r="H9" s="14">
         <v>90000</v>
@@ -4056,8 +4142,12 @@
       <c r="I9" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="45">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'Art Mod by Preva x Owlexandrea.jpg' WHERE id_produk = 9;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="14">
         <v>10</v>
       </c>
@@ -4077,7 +4167,7 @@
         <v>179</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="H10" s="14">
         <v>100000</v>
@@ -4085,8 +4175,12 @@
       <c r="I10" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="30">
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'zoo pod.jpg' WHERE id_produk = 10;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30">
       <c r="A11" s="14">
         <v>11</v>
       </c>
@@ -4106,7 +4200,7 @@
         <v>179</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="H11" s="14">
         <v>110000</v>
@@ -4114,8 +4208,12 @@
       <c r="I11" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="45">
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'caliburn.jpg' WHERE id_produk = 11;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45">
       <c r="A12" s="14">
         <v>12</v>
       </c>
@@ -4135,7 +4233,7 @@
         <v>179</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="H12" s="14">
         <v>120000</v>
@@ -4143,8 +4241,12 @@
       <c r="I12" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="30">
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'tesla terminator.jpg' WHERE id_produk = 12;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30">
       <c r="A13" s="14">
         <v>13</v>
       </c>
@@ -4164,7 +4266,7 @@
         <v>179</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="H13" s="14">
         <v>130000</v>
@@ -4172,8 +4274,12 @@
       <c r="I13" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="90">
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'smok rpm40.jpg' WHERE id_produk = 13;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45">
       <c r="A14" s="14">
         <v>14</v>
       </c>
@@ -4193,7 +4299,7 @@
         <v>179</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="H14" s="14">
         <v>140000</v>
@@ -4201,8 +4307,12 @@
       <c r="I14" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="30">
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'pico75watt.jpg' WHERE id_produk = 14;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30">
       <c r="A15" s="14">
         <v>15</v>
       </c>
@@ -4222,7 +4332,7 @@
         <v>179</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="H15" s="14">
         <v>150000</v>
@@ -4230,8 +4340,12 @@
       <c r="I15" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="45">
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'suorinair.jpg' WHERE id_produk = 15;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="45">
       <c r="A16" s="14">
         <v>16</v>
       </c>
@@ -4251,7 +4365,7 @@
         <v>179</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="H16" s="14">
         <v>160000</v>
@@ -4259,8 +4373,12 @@
       <c r="I16" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="90">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'druga squonk.jpg' WHERE id_produk = 16;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="45">
       <c r="A17" s="14">
         <v>17</v>
       </c>
@@ -4280,7 +4398,7 @@
         <v>179</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="H17" s="14">
         <v>170000</v>
@@ -4288,8 +4406,12 @@
       <c r="I17" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="60">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'Mecha Kit AV Timekeeper Revolver Kit.jpg' WHERE id_produk = 17;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45">
       <c r="A18" s="14">
         <v>18</v>
       </c>
@@ -4309,7 +4431,7 @@
         <v>179</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="H18" s="14">
         <v>20000</v>
@@ -4317,8 +4439,12 @@
       <c r="I18" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="45">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'smoant tc 218.jpg' WHERE id_produk = 18;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30">
       <c r="A19" s="14">
         <v>19</v>
       </c>
@@ -4338,7 +4464,7 @@
         <v>179</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="H19" s="14">
         <v>180000</v>
@@ -4346,8 +4472,12 @@
       <c r="I19" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="90">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'aegis legend.jpg' WHERE id_produk = 19;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="75">
       <c r="A20" s="14">
         <v>20</v>
       </c>
@@ -4367,7 +4497,7 @@
         <v>179</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="H20" s="14">
         <v>190000</v>
@@ -4375,8 +4505,12 @@
       <c r="I20" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="60">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'voopoo drag 2.jpg' WHERE id_produk = 20;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
       <c r="A21" s="14">
         <v>21</v>
       </c>
@@ -4395,9 +4529,7 @@
       <c r="F21" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>178</v>
-      </c>
+      <c r="G21" s="14"/>
       <c r="H21" s="14">
         <v>200000</v>
       </c>
@@ -4405,7 +4537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="45">
+    <row r="22" spans="1:11" ht="30">
       <c r="A22" s="14">
         <v>22</v>
       </c>
@@ -4424,9 +4556,7 @@
       <c r="F22" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G22" s="14" t="s">
-        <v>180</v>
-      </c>
+      <c r="G22" s="14"/>
       <c r="H22" s="14">
         <v>210000</v>
       </c>
@@ -4434,7 +4564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30">
+    <row r="23" spans="1:11" ht="30">
       <c r="A23" s="14">
         <v>23</v>
       </c>
@@ -4453,9 +4583,7 @@
       <c r="F23" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G23" s="14" t="s">
-        <v>181</v>
-      </c>
+      <c r="G23" s="14"/>
       <c r="H23" s="14">
         <v>220000</v>
       </c>
@@ -4463,7 +4591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="60">
+    <row r="24" spans="1:11" ht="45">
       <c r="A24" s="14">
         <v>24</v>
       </c>
@@ -4482,9 +4610,7 @@
       <c r="F24" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>182</v>
-      </c>
+      <c r="G24" s="14"/>
       <c r="H24" s="14">
         <v>230000</v>
       </c>
@@ -4492,7 +4618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="105">
+    <row r="25" spans="1:11" ht="75">
       <c r="A25" s="14">
         <v>25</v>
       </c>
@@ -4511,9 +4637,7 @@
       <c r="F25" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>183</v>
-      </c>
+      <c r="G25" s="14"/>
       <c r="H25" s="14">
         <v>240000</v>
       </c>
@@ -4521,7 +4645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30">
+    <row r="26" spans="1:11" ht="30">
       <c r="A26" s="14">
         <v>26</v>
       </c>
@@ -4540,9 +4664,7 @@
       <c r="F26" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>184</v>
-      </c>
+      <c r="G26" s="14"/>
       <c r="H26" s="14">
         <v>250000</v>
       </c>
@@ -4550,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="45">
+    <row r="27" spans="1:11" ht="30">
       <c r="A27" s="14">
         <v>27</v>
       </c>
@@ -4569,9 +4691,7 @@
       <c r="F27" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G27" s="14" t="s">
-        <v>185</v>
-      </c>
+      <c r="G27" s="14"/>
       <c r="H27" s="14">
         <v>260000</v>
       </c>
@@ -4579,7 +4699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="75">
+    <row r="28" spans="1:11" ht="45">
       <c r="A28" s="14">
         <v>28</v>
       </c>
@@ -4598,9 +4718,7 @@
       <c r="F28" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G28" s="14" t="s">
-        <v>186</v>
-      </c>
+      <c r="G28" s="14"/>
       <c r="H28" s="14">
         <v>270000</v>
       </c>
@@ -4608,7 +4726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="45">
+    <row r="29" spans="1:11" ht="45">
       <c r="A29" s="14">
         <v>29</v>
       </c>
@@ -4627,9 +4745,7 @@
       <c r="F29" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G29" s="14" t="s">
-        <v>187</v>
-      </c>
+      <c r="G29" s="14"/>
       <c r="H29" s="14">
         <v>280000</v>
       </c>
@@ -4637,7 +4753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30">
+    <row r="30" spans="1:11" ht="30">
       <c r="A30" s="14">
         <v>30</v>
       </c>
@@ -4657,7 +4773,7 @@
         <v>179</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="H30" s="14">
         <v>290000</v>
@@ -4665,8 +4781,12 @@
       <c r="I30" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="45">
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'caliburn.jpg' WHERE id_produk = 30;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="45">
       <c r="A31" s="14">
         <v>31</v>
       </c>
@@ -4685,9 +4805,7 @@
       <c r="F31" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G31" s="14" t="s">
-        <v>189</v>
-      </c>
+      <c r="G31" s="14"/>
       <c r="H31" s="14">
         <v>300000</v>
       </c>
@@ -4695,7 +4813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30">
+    <row r="32" spans="1:11" ht="30">
       <c r="A32" s="14">
         <v>32</v>
       </c>
@@ -4714,9 +4832,7 @@
       <c r="F32" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G32" s="14" t="s">
-        <v>190</v>
-      </c>
+      <c r="G32" s="14"/>
       <c r="H32" s="14">
         <v>310000</v>
       </c>
@@ -4724,7 +4840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="90">
+    <row r="33" spans="1:9" ht="45">
       <c r="A33" s="14">
         <v>33</v>
       </c>
@@ -4743,9 +4859,7 @@
       <c r="F33" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G33" s="14" t="s">
-        <v>191</v>
-      </c>
+      <c r="G33" s="14"/>
       <c r="H33" s="14">
         <v>320000</v>
       </c>
@@ -4772,9 +4886,7 @@
       <c r="F34" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G34" s="14" t="s">
-        <v>192</v>
-      </c>
+      <c r="G34" s="14"/>
       <c r="H34" s="14">
         <v>340000</v>
       </c>
@@ -4782,7 +4894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="45">
+    <row r="35" spans="1:9" ht="30">
       <c r="A35" s="14">
         <v>35</v>
       </c>
@@ -4801,9 +4913,7 @@
       <c r="F35" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G35" s="14" t="s">
-        <v>193</v>
-      </c>
+      <c r="G35" s="14"/>
       <c r="H35" s="14">
         <v>350000</v>
       </c>
@@ -4811,7 +4921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="90">
+    <row r="36" spans="1:9" ht="45">
       <c r="A36" s="14">
         <v>36</v>
       </c>
@@ -4830,9 +4940,7 @@
       <c r="F36" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G36" s="14" t="s">
-        <v>194</v>
-      </c>
+      <c r="G36" s="14"/>
       <c r="H36" s="14">
         <v>360000</v>
       </c>
@@ -4840,7 +4948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="60">
+    <row r="37" spans="1:9" ht="45">
       <c r="A37" s="14">
         <v>37</v>
       </c>
@@ -4859,9 +4967,7 @@
       <c r="F37" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G37" s="14" t="s">
-        <v>195</v>
-      </c>
+      <c r="G37" s="14"/>
       <c r="H37" s="14">
         <v>370000</v>
       </c>
@@ -4869,7 +4975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="45">
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="14">
         <v>38</v>
       </c>
@@ -4888,9 +4994,7 @@
       <c r="F38" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G38" s="14" t="s">
-        <v>196</v>
-      </c>
+      <c r="G38" s="14"/>
       <c r="H38" s="14">
         <v>380000</v>
       </c>
@@ -4898,7 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="90">
+    <row r="39" spans="1:9" ht="75">
       <c r="A39" s="14">
         <v>39</v>
       </c>
@@ -4917,9 +5021,7 @@
       <c r="F39" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G39" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="G39" s="14"/>
       <c r="H39" s="14">
         <v>380000</v>
       </c>
@@ -4927,7 +5029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="60">
+    <row r="40" spans="1:9" ht="30">
       <c r="A40" s="14">
         <v>40</v>
       </c>
@@ -4946,9 +5048,7 @@
       <c r="F40" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G40" s="14" t="s">
-        <v>178</v>
-      </c>
+      <c r="G40" s="14"/>
       <c r="H40" s="14">
         <v>390000</v>
       </c>
@@ -4956,7 +5056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="45">
+    <row r="41" spans="1:9" ht="30">
       <c r="A41" s="14">
         <v>41</v>
       </c>
@@ -4975,9 +5075,7 @@
       <c r="F41" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G41" s="14" t="s">
-        <v>180</v>
-      </c>
+      <c r="G41" s="14"/>
       <c r="H41" s="14">
         <v>400000</v>
       </c>
@@ -5004,9 +5102,7 @@
       <c r="F42" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G42" s="14" t="s">
-        <v>181</v>
-      </c>
+      <c r="G42" s="14"/>
       <c r="H42" s="14">
         <v>410000</v>
       </c>
@@ -5014,7 +5110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="60">
+    <row r="43" spans="1:9" ht="45">
       <c r="A43" s="14">
         <v>43</v>
       </c>
@@ -5033,9 +5129,7 @@
       <c r="F43" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G43" s="14" t="s">
-        <v>182</v>
-      </c>
+      <c r="G43" s="14"/>
       <c r="H43" s="14">
         <v>420000</v>
       </c>
@@ -5043,7 +5137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="105">
+    <row r="44" spans="1:9" ht="75">
       <c r="A44" s="14">
         <v>44</v>
       </c>
@@ -5062,9 +5156,7 @@
       <c r="F44" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G44" s="14" t="s">
-        <v>183</v>
-      </c>
+      <c r="G44" s="14"/>
       <c r="H44" s="14">
         <v>430000</v>
       </c>
@@ -5091,9 +5183,7 @@
       <c r="F45" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G45" s="14" t="s">
-        <v>184</v>
-      </c>
+      <c r="G45" s="14"/>
       <c r="H45" s="14">
         <v>440000</v>
       </c>
@@ -5101,7 +5191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="45">
+    <row r="46" spans="1:9" ht="30">
       <c r="A46" s="14">
         <v>46</v>
       </c>
@@ -5120,9 +5210,7 @@
       <c r="F46" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G46" s="14" t="s">
-        <v>185</v>
-      </c>
+      <c r="G46" s="14"/>
       <c r="H46" s="14">
         <v>450000</v>
       </c>
@@ -5130,7 +5218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="75">
+    <row r="47" spans="1:9" ht="45">
       <c r="A47" s="14">
         <v>47</v>
       </c>
@@ -5149,9 +5237,7 @@
       <c r="F47" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G47" s="14" t="s">
-        <v>186</v>
-      </c>
+      <c r="G47" s="14"/>
       <c r="H47" s="14">
         <v>460000</v>
       </c>
@@ -5178,9 +5264,7 @@
       <c r="F48" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G48" s="14" t="s">
-        <v>187</v>
-      </c>
+      <c r="G48" s="14"/>
       <c r="H48" s="14">
         <v>470000</v>
       </c>
@@ -5207,9 +5291,7 @@
       <c r="F49" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G49" s="14" t="s">
-        <v>188</v>
-      </c>
+      <c r="G49" s="14"/>
       <c r="H49" s="14">
         <v>480000</v>
       </c>
@@ -5236,9 +5318,7 @@
       <c r="F50" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G50" s="14" t="s">
-        <v>189</v>
-      </c>
+      <c r="G50" s="14"/>
       <c r="H50" s="14">
         <v>490000</v>
       </c>
@@ -5265,9 +5345,7 @@
       <c r="F51" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G51" s="14" t="s">
-        <v>190</v>
-      </c>
+      <c r="G51" s="14"/>
       <c r="H51" s="14">
         <v>500000</v>
       </c>
@@ -5294,9 +5372,7 @@
       <c r="F52" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="G52" s="14" t="s">
-        <v>200</v>
-      </c>
+      <c r="G52" s="14"/>
       <c r="H52" s="14">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
2022 08 14 11:22
</commit_message>
<xml_diff>
--- a/assets/datamentah.xlsx
+++ b/assets/datamentah.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19590" windowHeight="7830" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19590" windowHeight="7830" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="bank" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="clear" sheetId="4" r:id="rId7"/>
     <sheet name="produk" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="227">
   <si>
     <t>id_bank</t>
   </si>
@@ -717,7 +718,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -3838,7 +3839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -3883,7 +3884,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45">
+    <row r="2" spans="1:11" ht="30">
       <c r="A2" s="14">
         <v>2</v>
       </c>
@@ -4345,7 +4346,7 @@
         <v>UPDATE produk SET gambar = 'suorinair.jpg' WHERE id_produk = 15;</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="45">
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="14">
         <v>16</v>
       </c>
@@ -5394,4 +5395,599 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60">
+      <c r="A2" s="14">
+        <v>2</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
+        <v>20</v>
+      </c>
+      <c r="E2" s="14">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" s="14">
+        <v>20000</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45">
+      <c r="A3" s="14">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>20</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="H3" s="14">
+        <v>30000</v>
+      </c>
+      <c r="I3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4" s="14">
+        <v>4</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="14">
+        <v>3</v>
+      </c>
+      <c r="D4" s="14">
+        <v>20</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H4" s="14">
+        <v>40000</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60">
+      <c r="A5" s="14">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="14">
+        <v>4</v>
+      </c>
+      <c r="D5" s="14">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="14">
+        <v>50000</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="105">
+      <c r="A6" s="14">
+        <v>6</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="14">
+        <v>5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="H6" s="14">
+        <v>60000</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30">
+      <c r="A7" s="14">
+        <v>7</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>20</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="H7" s="14">
+        <v>70000</v>
+      </c>
+      <c r="I7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45">
+      <c r="A8" s="14">
+        <v>8</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>20</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="14">
+        <v>80000</v>
+      </c>
+      <c r="I8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75">
+      <c r="A9" s="14">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="14">
+        <v>3</v>
+      </c>
+      <c r="D9" s="14">
+        <v>20</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="H9" s="14">
+        <v>90000</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45">
+      <c r="A10" s="14">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="14">
+        <v>4</v>
+      </c>
+      <c r="D10" s="14">
+        <v>20</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="H10" s="14">
+        <v>100000</v>
+      </c>
+      <c r="I10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="14">
+        <v>11</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="14">
+        <v>5</v>
+      </c>
+      <c r="D11" s="14">
+        <v>20</v>
+      </c>
+      <c r="E11" s="14">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="H11" s="14">
+        <v>110000</v>
+      </c>
+      <c r="I11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45">
+      <c r="A12" s="14">
+        <v>12</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
+        <v>20</v>
+      </c>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="H12" s="14">
+        <v>120000</v>
+      </c>
+      <c r="I12" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45">
+      <c r="A13" s="14">
+        <v>13</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="14">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14">
+        <v>20</v>
+      </c>
+      <c r="E13" s="14">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="H13" s="14">
+        <v>130000</v>
+      </c>
+      <c r="I13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="90">
+      <c r="A14" s="14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="14">
+        <v>20</v>
+      </c>
+      <c r="E14" s="14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14" s="14">
+        <v>140000</v>
+      </c>
+      <c r="I14" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30">
+      <c r="A15" s="14">
+        <v>15</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="14">
+        <v>4</v>
+      </c>
+      <c r="D15" s="14">
+        <v>20</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="H15" s="14">
+        <v>150000</v>
+      </c>
+      <c r="I15" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45">
+      <c r="A16" s="14">
+        <v>16</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="14">
+        <v>5</v>
+      </c>
+      <c r="D16" s="14">
+        <v>20</v>
+      </c>
+      <c r="E16" s="14">
+        <v>1</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="H16" s="14">
+        <v>160000</v>
+      </c>
+      <c r="I16" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="90">
+      <c r="A17" s="14">
+        <v>17</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>20</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="H17" s="14">
+        <v>170000</v>
+      </c>
+      <c r="I17" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60">
+      <c r="A18" s="14">
+        <v>18</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2</v>
+      </c>
+      <c r="D18" s="14">
+        <v>20</v>
+      </c>
+      <c r="E18" s="14">
+        <v>1</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="H18" s="14">
+        <v>20000</v>
+      </c>
+      <c r="I18" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45">
+      <c r="A19" s="14">
+        <v>19</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="14">
+        <v>3</v>
+      </c>
+      <c r="D19" s="14">
+        <v>20</v>
+      </c>
+      <c r="E19" s="14">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="H19" s="14">
+        <v>180000</v>
+      </c>
+      <c r="I19" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="90">
+      <c r="A20" s="14">
+        <v>20</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" s="14">
+        <v>4</v>
+      </c>
+      <c r="D20" s="14">
+        <v>20</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="H20" s="14">
+        <v>190000</v>
+      </c>
+      <c r="I20" s="14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2022 08 14 13:50
</commit_message>
<xml_diff>
--- a/assets/datamentah.xlsx
+++ b/assets/datamentah.xlsx
@@ -20,8 +20,12 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="clear" sheetId="4" r:id="rId7"/>
     <sheet name="produk" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Sheet2!$A$1:$I$52</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="238">
   <si>
     <t>id_bank</t>
   </si>
@@ -713,13 +717,161 @@
   </si>
   <si>
     <t>Mecha Kit AV Timekeeper Revolver Kit.jpg</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">baterai awt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>26650.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">baterai vrk </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>18650.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">batre sony vtc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>6a.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">FAQ funky </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>monkey.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">kapas holy </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>fiber.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">kapas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>kendo.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>oatdrips.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>rda hadaly sxkjpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">rta fatality </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>25mm.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>tokyoman.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>upods cube.jpeg</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,6 +915,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -813,7 +969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -844,6 +1000,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1297,6 +1456,601 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60">
+      <c r="A2" s="14">
+        <v>2</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
+        <v>20</v>
+      </c>
+      <c r="E2" s="14">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" s="14">
+        <v>20000</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45">
+      <c r="A3" s="14">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>20</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="H3" s="14">
+        <v>30000</v>
+      </c>
+      <c r="I3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4" s="14">
+        <v>4</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="14">
+        <v>3</v>
+      </c>
+      <c r="D4" s="14">
+        <v>20</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H4" s="14">
+        <v>40000</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60">
+      <c r="A5" s="14">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="14">
+        <v>4</v>
+      </c>
+      <c r="D5" s="14">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="14">
+        <v>50000</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="105">
+      <c r="A6" s="14">
+        <v>6</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="14">
+        <v>5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="H6" s="14">
+        <v>60000</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30">
+      <c r="A7" s="14">
+        <v>7</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>20</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="H7" s="14">
+        <v>70000</v>
+      </c>
+      <c r="I7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45">
+      <c r="A8" s="14">
+        <v>8</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>20</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="14">
+        <v>80000</v>
+      </c>
+      <c r="I8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75">
+      <c r="A9" s="14">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="14">
+        <v>3</v>
+      </c>
+      <c r="D9" s="14">
+        <v>20</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="H9" s="14">
+        <v>90000</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45">
+      <c r="A10" s="14">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="14">
+        <v>4</v>
+      </c>
+      <c r="D10" s="14">
+        <v>20</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="H10" s="14">
+        <v>100000</v>
+      </c>
+      <c r="I10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="14">
+        <v>11</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="14">
+        <v>5</v>
+      </c>
+      <c r="D11" s="14">
+        <v>20</v>
+      </c>
+      <c r="E11" s="14">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="H11" s="14">
+        <v>110000</v>
+      </c>
+      <c r="I11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45">
+      <c r="A12" s="14">
+        <v>12</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
+        <v>20</v>
+      </c>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="H12" s="14">
+        <v>120000</v>
+      </c>
+      <c r="I12" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45">
+      <c r="A13" s="14">
+        <v>13</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="14">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14">
+        <v>20</v>
+      </c>
+      <c r="E13" s="14">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="H13" s="14">
+        <v>130000</v>
+      </c>
+      <c r="I13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="90">
+      <c r="A14" s="14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="14">
+        <v>20</v>
+      </c>
+      <c r="E14" s="14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14" s="14">
+        <v>140000</v>
+      </c>
+      <c r="I14" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30">
+      <c r="A15" s="14">
+        <v>15</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="14">
+        <v>4</v>
+      </c>
+      <c r="D15" s="14">
+        <v>20</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="H15" s="14">
+        <v>150000</v>
+      </c>
+      <c r="I15" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45">
+      <c r="A16" s="14">
+        <v>16</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="14">
+        <v>5</v>
+      </c>
+      <c r="D16" s="14">
+        <v>20</v>
+      </c>
+      <c r="E16" s="14">
+        <v>1</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="H16" s="14">
+        <v>160000</v>
+      </c>
+      <c r="I16" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="90">
+      <c r="A17" s="14">
+        <v>17</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>20</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="H17" s="14">
+        <v>170000</v>
+      </c>
+      <c r="I17" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60">
+      <c r="A18" s="14">
+        <v>18</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2</v>
+      </c>
+      <c r="D18" s="14">
+        <v>20</v>
+      </c>
+      <c r="E18" s="14">
+        <v>1</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="H18" s="14">
+        <v>20000</v>
+      </c>
+      <c r="I18" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45">
+      <c r="A19" s="14">
+        <v>19</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="14">
+        <v>3</v>
+      </c>
+      <c r="D19" s="14">
+        <v>20</v>
+      </c>
+      <c r="E19" s="14">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="H19" s="14">
+        <v>180000</v>
+      </c>
+      <c r="I19" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="90">
+      <c r="A20" s="14">
+        <v>20</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" s="14">
+        <v>4</v>
+      </c>
+      <c r="D20" s="14">
+        <v>20</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="H20" s="14">
+        <v>190000</v>
+      </c>
+      <c r="I20" s="14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -3840,7 +4594,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3946,7 +4700,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K30" si="0">"UPDATE produk SET gambar = '"&amp;G3&amp;"' WHERE id_produk = "&amp;A3&amp;";"</f>
+        <f t="shared" ref="K2:K30" si="0">"UPDATE produk SET gambar = '"&amp;G3&amp;"' WHERE id_produk = "&amp;A3&amp;";"</f>
         <v>UPDATE produk SET gambar = 'exceed grip.jpg' WHERE id_produk = 3;</v>
       </c>
     </row>
@@ -5399,13 +6153,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="15" t="s">
@@ -5436,7 +6194,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60">
+    <row r="2" spans="1:9" ht="60" hidden="1">
       <c r="A2" s="14">
         <v>2</v>
       </c>
@@ -5465,7 +6223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45">
+    <row r="3" spans="1:9" ht="45" hidden="1">
       <c r="A3" s="14">
         <v>3</v>
       </c>
@@ -5494,7 +6252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30">
+    <row r="4" spans="1:9" ht="30" hidden="1">
       <c r="A4" s="14">
         <v>4</v>
       </c>
@@ -5523,7 +6281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60">
+    <row r="5" spans="1:9" ht="60" hidden="1">
       <c r="A5" s="14">
         <v>5</v>
       </c>
@@ -5552,7 +6310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="105">
+    <row r="6" spans="1:9" ht="105" hidden="1">
       <c r="A6" s="14">
         <v>6</v>
       </c>
@@ -5581,7 +6339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30">
+    <row r="7" spans="1:9" ht="30" hidden="1">
       <c r="A7" s="14">
         <v>7</v>
       </c>
@@ -5610,7 +6368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45">
+    <row r="8" spans="1:9" ht="45" hidden="1">
       <c r="A8" s="14">
         <v>8</v>
       </c>
@@ -5639,7 +6397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="75">
+    <row r="9" spans="1:9" ht="75" hidden="1">
       <c r="A9" s="14">
         <v>9</v>
       </c>
@@ -5668,7 +6426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45">
+    <row r="10" spans="1:9" ht="45" hidden="1">
       <c r="A10" s="14">
         <v>10</v>
       </c>
@@ -5697,7 +6455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30">
+    <row r="11" spans="1:9" ht="30" hidden="1">
       <c r="A11" s="14">
         <v>11</v>
       </c>
@@ -5726,7 +6484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45">
+    <row r="12" spans="1:9" ht="45" hidden="1">
       <c r="A12" s="14">
         <v>12</v>
       </c>
@@ -5755,7 +6513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="45">
+    <row r="13" spans="1:9" ht="45" hidden="1">
       <c r="A13" s="14">
         <v>13</v>
       </c>
@@ -5784,7 +6542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="90">
+    <row r="14" spans="1:9" ht="90" hidden="1">
       <c r="A14" s="14">
         <v>14</v>
       </c>
@@ -5813,7 +6571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30">
+    <row r="15" spans="1:9" ht="30" hidden="1">
       <c r="A15" s="14">
         <v>15</v>
       </c>
@@ -5842,7 +6600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="45">
+    <row r="16" spans="1:9" ht="45" hidden="1">
       <c r="A16" s="14">
         <v>16</v>
       </c>
@@ -5871,7 +6629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="90">
+    <row r="17" spans="1:12" ht="90" hidden="1">
       <c r="A17" s="14">
         <v>17</v>
       </c>
@@ -5900,7 +6658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="60">
+    <row r="18" spans="1:12" ht="60" hidden="1">
       <c r="A18" s="14">
         <v>18</v>
       </c>
@@ -5929,7 +6687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45">
+    <row r="19" spans="1:12" ht="45" hidden="1">
       <c r="A19" s="14">
         <v>19</v>
       </c>
@@ -5958,7 +6716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="90">
+    <row r="20" spans="1:12" ht="90" hidden="1">
       <c r="A20" s="14">
         <v>20</v>
       </c>
@@ -5987,7 +6745,978 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21" spans="1:12" ht="60">
+      <c r="A21" s="14">
+        <v>21</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="14">
+        <v>5</v>
+      </c>
+      <c r="D21" s="14">
+        <v>20</v>
+      </c>
+      <c r="E21" s="14">
+        <v>1</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="H21" s="14">
+        <v>200000</v>
+      </c>
+      <c r="I21" s="14">
+        <v>1</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" ref="K21:L29" si="0">"UPDATE produk SET gambar = '"&amp;G2&amp;"' WHERE id_produk = "&amp;A21&amp;";"</f>
+        <v>UPDATE produk SET gambar = 'dovpo panda.jpg' WHERE id_produk = 21;</v>
+      </c>
+      <c r="L21" t="str">
+        <f>"UPDATE produk SET nama_produk = '"&amp;G21&amp;"' WHERE id_produk = "&amp;A21&amp;";"</f>
+        <v>UPDATE produk SET nama_produk = 'baterai awt 26650.jpg' WHERE id_produk = 21;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="45">
+      <c r="A22" s="14">
+        <v>22</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1</v>
+      </c>
+      <c r="D22" s="14">
+        <v>20</v>
+      </c>
+      <c r="E22" s="14">
+        <v>1</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="H22" s="14">
+        <v>210000</v>
+      </c>
+      <c r="I22" s="14">
+        <v>1</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'exceed grip.jpg' WHERE id_produk = 22;</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" ref="L22:L31" si="1">"UPDATE produk SET nama_produk = '"&amp;G22&amp;"' WHERE id_produk = "&amp;A22&amp;";"</f>
+        <v>UPDATE produk SET nama_produk = 'baterai vrk 18650.jpg' WHERE id_produk = 22;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30">
+      <c r="A23" s="14">
+        <v>23</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="14">
+        <v>2</v>
+      </c>
+      <c r="D23" s="14">
+        <v>20</v>
+      </c>
+      <c r="E23" s="14">
+        <v>1</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="H23" s="14">
+        <v>220000</v>
+      </c>
+      <c r="I23" s="14">
+        <v>1</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'Upods Cube,jpg' WHERE id_produk = 23;</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE produk SET nama_produk = 'batre sony vtc 6a.jpg' WHERE id_produk = 23;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="60">
+      <c r="A24" s="14">
+        <v>24</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="14">
+        <v>3</v>
+      </c>
+      <c r="D24" s="14">
+        <v>20</v>
+      </c>
+      <c r="E24" s="14">
+        <v>1</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="H24" s="14">
+        <v>230000</v>
+      </c>
+      <c r="I24" s="14">
+        <v>1</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'vaporite mecha kit 22.jpg' WHERE id_produk = 24;</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE produk SET nama_produk = 'FAQ funky monkey.jpg' WHERE id_produk = 24;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="105">
+      <c r="A25" s="14">
+        <v>25</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="14">
+        <v>4</v>
+      </c>
+      <c r="D25" s="14">
+        <v>20</v>
+      </c>
+      <c r="E25" s="14">
+        <v>1</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="H25" s="14">
+        <v>240000</v>
+      </c>
+      <c r="I25" s="14">
+        <v>1</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'hexohm v3.jpg' WHERE id_produk = 25;</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE produk SET nama_produk = 'kapas holy fiber.jpg' WHERE id_produk = 25;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="30">
+      <c r="A26" s="14">
+        <v>26</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="14">
+        <v>5</v>
+      </c>
+      <c r="D26" s="14">
+        <v>20</v>
+      </c>
+      <c r="E26" s="14">
+        <v>1</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="H26" s="14">
+        <v>250000</v>
+      </c>
+      <c r="I26" s="14">
+        <v>1</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'juul.jpg' WHERE id_produk = 26;</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE produk SET nama_produk = 'kapas kendo.jpg' WHERE id_produk = 26;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="45">
+      <c r="A27" s="14">
+        <v>27</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1</v>
+      </c>
+      <c r="D27" s="14">
+        <v>20</v>
+      </c>
+      <c r="E27" s="14">
+        <v>1</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H27" s="14">
+        <v>260000</v>
+      </c>
+      <c r="I27" s="14">
+        <v>1</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'smok fetch mini.jpg' WHERE id_produk = 27;</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE produk SET nama_produk = 'oatdrips.jpg' WHERE id_produk = 27;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="75">
+      <c r="A28" s="14">
+        <v>28</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" s="14">
+        <v>2</v>
+      </c>
+      <c r="D28" s="14">
+        <v>20</v>
+      </c>
+      <c r="E28" s="14">
+        <v>1</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="H28" s="14">
+        <v>270000</v>
+      </c>
+      <c r="I28" s="14">
+        <v>1</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'Art Mod by Preva x Owlexandrea.jpg' WHERE id_produk = 28;</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE produk SET nama_produk = 'rda hadaly sxkjpg' WHERE id_produk = 28;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="45">
+      <c r="A29" s="14">
+        <v>29</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29" s="14">
+        <v>3</v>
+      </c>
+      <c r="D29" s="14">
+        <v>20</v>
+      </c>
+      <c r="E29" s="14">
+        <v>1</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="H29" s="14">
+        <v>280000</v>
+      </c>
+      <c r="I29" s="14">
+        <v>1</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE produk SET gambar = 'zoo pod.jpg' WHERE id_produk = 29;</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE produk SET nama_produk = 'rta fatality 25mm.jpg' WHERE id_produk = 29;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30" hidden="1">
+      <c r="A30" s="14">
+        <v>30</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" s="14">
+        <v>4</v>
+      </c>
+      <c r="D30" s="14">
+        <v>20</v>
+      </c>
+      <c r="E30" s="14">
+        <v>1</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="H30" s="14">
+        <v>290000</v>
+      </c>
+      <c r="I30" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="45">
+      <c r="A31" s="14">
+        <v>31</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="14">
+        <v>5</v>
+      </c>
+      <c r="D31" s="14">
+        <v>20</v>
+      </c>
+      <c r="E31" s="14">
+        <v>1</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="H31" s="14">
+        <v>300000</v>
+      </c>
+      <c r="I31" s="14">
+        <v>1</v>
+      </c>
+      <c r="K31" t="str">
+        <f>"UPDATE produk SET gambar = '"&amp;G12&amp;"' WHERE id_produk = "&amp;A31&amp;";"</f>
+        <v>UPDATE produk SET gambar = 'tesla terminator.jpg' WHERE id_produk = 31;</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE produk SET nama_produk = 'upods cube.jpeg' WHERE id_produk = 31;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="30">
+      <c r="A32" s="14">
+        <v>32</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" s="14">
+        <v>1</v>
+      </c>
+      <c r="D32" s="14">
+        <v>20</v>
+      </c>
+      <c r="E32" s="14">
+        <v>1</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14">
+        <v>310000</v>
+      </c>
+      <c r="I32" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="90">
+      <c r="A33" s="14">
+        <v>33</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" s="14">
+        <v>2</v>
+      </c>
+      <c r="D33" s="14">
+        <v>20</v>
+      </c>
+      <c r="E33" s="14">
+        <v>1</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14">
+        <v>320000</v>
+      </c>
+      <c r="I33" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30">
+      <c r="A34" s="14">
+        <v>34</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" s="14">
+        <v>3</v>
+      </c>
+      <c r="D34" s="14">
+        <v>20</v>
+      </c>
+      <c r="E34" s="14">
+        <v>1</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14">
+        <v>340000</v>
+      </c>
+      <c r="I34" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="45">
+      <c r="A35" s="14">
+        <v>35</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C35" s="14">
+        <v>4</v>
+      </c>
+      <c r="D35" s="14">
+        <v>20</v>
+      </c>
+      <c r="E35" s="14">
+        <v>1</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14">
+        <v>350000</v>
+      </c>
+      <c r="I35" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="90">
+      <c r="A36" s="14">
+        <v>36</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" s="14">
+        <v>5</v>
+      </c>
+      <c r="D36" s="14">
+        <v>20</v>
+      </c>
+      <c r="E36" s="14">
+        <v>1</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14">
+        <v>360000</v>
+      </c>
+      <c r="I36" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="60">
+      <c r="A37" s="14">
+        <v>37</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" s="14">
+        <v>1</v>
+      </c>
+      <c r="D37" s="14">
+        <v>20</v>
+      </c>
+      <c r="E37" s="14">
+        <v>1</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14">
+        <v>370000</v>
+      </c>
+      <c r="I37" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="45">
+      <c r="A38" s="14">
+        <v>38</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C38" s="14">
+        <v>2</v>
+      </c>
+      <c r="D38" s="14">
+        <v>20</v>
+      </c>
+      <c r="E38" s="14">
+        <v>1</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14">
+        <v>380000</v>
+      </c>
+      <c r="I38" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="90">
+      <c r="A39" s="14">
+        <v>39</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="14">
+        <v>3</v>
+      </c>
+      <c r="D39" s="14">
+        <v>20</v>
+      </c>
+      <c r="E39" s="14">
+        <v>1</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14">
+        <v>380000</v>
+      </c>
+      <c r="I39" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60">
+      <c r="A40" s="14">
+        <v>40</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="14">
+        <v>4</v>
+      </c>
+      <c r="D40" s="14">
+        <v>20</v>
+      </c>
+      <c r="E40" s="14">
+        <v>1</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14">
+        <v>390000</v>
+      </c>
+      <c r="I40" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="45">
+      <c r="A41" s="14">
+        <v>41</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" s="14">
+        <v>5</v>
+      </c>
+      <c r="D41" s="14">
+        <v>20</v>
+      </c>
+      <c r="E41" s="14">
+        <v>1</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14">
+        <v>400000</v>
+      </c>
+      <c r="I41" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30">
+      <c r="A42" s="14">
+        <v>42</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="14">
+        <v>1</v>
+      </c>
+      <c r="D42" s="14">
+        <v>20</v>
+      </c>
+      <c r="E42" s="14">
+        <v>1</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14">
+        <v>410000</v>
+      </c>
+      <c r="I42" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="60">
+      <c r="A43" s="14">
+        <v>43</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" s="14">
+        <v>2</v>
+      </c>
+      <c r="D43" s="14">
+        <v>20</v>
+      </c>
+      <c r="E43" s="14">
+        <v>1</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14">
+        <v>420000</v>
+      </c>
+      <c r="I43" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="105">
+      <c r="A44" s="14">
+        <v>44</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="14">
+        <v>3</v>
+      </c>
+      <c r="D44" s="14">
+        <v>20</v>
+      </c>
+      <c r="E44" s="14">
+        <v>1</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14">
+        <v>430000</v>
+      </c>
+      <c r="I44" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30">
+      <c r="A45" s="14">
+        <v>45</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="14">
+        <v>4</v>
+      </c>
+      <c r="D45" s="14">
+        <v>20</v>
+      </c>
+      <c r="E45" s="14">
+        <v>1</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14">
+        <v>440000</v>
+      </c>
+      <c r="I45" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="45">
+      <c r="A46" s="14">
+        <v>46</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="14">
+        <v>5</v>
+      </c>
+      <c r="D46" s="14">
+        <v>20</v>
+      </c>
+      <c r="E46" s="14">
+        <v>1</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14">
+        <v>450000</v>
+      </c>
+      <c r="I46" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="75">
+      <c r="A47" s="14">
+        <v>47</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="14">
+        <v>1</v>
+      </c>
+      <c r="D47" s="14">
+        <v>20</v>
+      </c>
+      <c r="E47" s="14">
+        <v>1</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14">
+        <v>460000</v>
+      </c>
+      <c r="I47" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="45">
+      <c r="A48" s="14">
+        <v>48</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" s="14">
+        <v>2</v>
+      </c>
+      <c r="D48" s="14">
+        <v>20</v>
+      </c>
+      <c r="E48" s="14">
+        <v>1</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14">
+        <v>470000</v>
+      </c>
+      <c r="I48" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30">
+      <c r="A49" s="14">
+        <v>49</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="14">
+        <v>3</v>
+      </c>
+      <c r="D49" s="14">
+        <v>20</v>
+      </c>
+      <c r="E49" s="14">
+        <v>1</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14">
+        <v>480000</v>
+      </c>
+      <c r="I49" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="45">
+      <c r="A50" s="14">
+        <v>50</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="14">
+        <v>4</v>
+      </c>
+      <c r="D50" s="14">
+        <v>20</v>
+      </c>
+      <c r="E50" s="14">
+        <v>1</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14">
+        <v>490000</v>
+      </c>
+      <c r="I50" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30">
+      <c r="A51" s="14">
+        <v>51</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="14">
+        <v>5</v>
+      </c>
+      <c r="D51" s="14">
+        <v>20</v>
+      </c>
+      <c r="E51" s="14">
+        <v>1</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14">
+        <v>500000</v>
+      </c>
+      <c r="I51" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="45">
+      <c r="A52" s="14">
+        <v>53</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C52" s="14">
+        <v>2</v>
+      </c>
+      <c r="D52" s="14">
+        <v>200</v>
+      </c>
+      <c r="E52" s="14">
+        <v>0</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14">
+        <v>200</v>
+      </c>
+      <c r="I52" s="14">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I52">
+    <filterColumn colId="6">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>